<commit_message>
Reading in params from excel
</commit_message>
<xml_diff>
--- a/config_files/State_Conversion.xlsx
+++ b/config_files/State_Conversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsakG\projects\exjobb\config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0DE8D5-1B89-4C4A-BAB9-F3F09A4FBA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840FDB9C-397A-47A8-B541-E50754514FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43200" yWindow="-90" windowWidth="14400" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StartingState" sheetId="1" r:id="rId1"/>
@@ -61,10 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
-  <si>
-    <t xml:space="preserve">Technology </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>ai_ml</t>
   </si>
@@ -160,9 +157,6 @@
   </si>
   <si>
     <t>PlayerB_y</t>
-  </si>
-  <si>
-    <t>ConversionMatrix</t>
   </si>
   <si>
     <t>Phi, Psi</t>
@@ -504,9 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -516,19 +508,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
       <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
         <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -540,7 +529,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -551,7 +540,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -562,7 +551,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -573,7 +562,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -584,7 +573,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -595,7 +584,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -606,7 +595,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -617,7 +606,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -628,7 +617,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -639,7 +628,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -657,9 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D0BDA4-F073-4C1B-804A-348F3CB1E796}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -667,9 +654,6 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1:L1">TRANSPOSE(StartingState!A2:A12)</f>
         <v>sen_tec</v>
@@ -707,7 +691,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -745,7 +729,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -783,7 +767,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -821,7 +805,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -859,7 +843,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -897,7 +881,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>9</v>
@@ -935,7 +919,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -973,7 +957,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1051,7 +1035,7 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1:L1">TRANSPOSE(StartingState!A2:A12)</f>
@@ -1088,33 +1072,33 @@
         <v>sim_mod</v>
       </c>
       <c r="O1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>22</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>23</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>24</v>
-      </c>
-      <c r="X1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1169,7 +1153,7 @@
         <v>0.95257412682243336</v>
       </c>
       <c r="T2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U2" s="2" cm="1">
         <f t="array" ref="U2:V9">(1 + MMULT(B2:L9*B14,Q2:R12)) * W2:X9</f>
@@ -1187,7 +1171,7 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -1240,7 +1224,7 @@
         <v>4.7425873177566781E-2</v>
       </c>
       <c r="T3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U3" s="3">
         <v>32.346954843538882</v>
@@ -1257,7 +1241,7 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1310,7 +1294,7 @@
         <v>0.99330714907571527</v>
       </c>
       <c r="T4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="U4" s="1">
         <v>6.8624956952355376</v>
@@ -1327,7 +1311,7 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1380,7 +1364,7 @@
         <v>0.7310585786300049</v>
       </c>
       <c r="T5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U5" s="3">
         <v>1.8412250628948656</v>
@@ -1397,7 +1381,7 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -1450,7 +1434,7 @@
         <v>0.2689414213699951</v>
       </c>
       <c r="T6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U6" s="1">
         <v>6.6235971934235218</v>
@@ -1467,7 +1451,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>9</v>
@@ -1520,7 +1504,7 @@
         <v>0.7310585786300049</v>
       </c>
       <c r="T7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U7" s="3">
         <v>1.9984762428218481</v>
@@ -1537,7 +1521,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1590,7 +1574,7 @@
         <v>0.99330714907571527</v>
       </c>
       <c r="T8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U8" s="2">
         <v>0.5</v>
@@ -1607,7 +1591,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1660,7 +1644,7 @@
         <v>0.7310585786300049</v>
       </c>
       <c r="T9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U9" s="2">
         <v>1</v>
@@ -1715,7 +1699,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -1740,7 +1724,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1748,7 +1732,7 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1">
         <v>0.1</v>

</xml_diff>

<commit_message>
Fixed battle function. Now iterative.
</commit_message>
<xml_diff>
--- a/config_files/State_Conversion.xlsx
+++ b/config_files/State_Conversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsakG\projects\exjobb\config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429C16A8-DF5A-42DC-9FE0-6436E1194C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8A673F-E55E-462D-AAE4-021CCF4B0D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31920" yWindow="3030" windowWidth="21600" windowHeight="12735" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StartingState" sheetId="1" r:id="rId1"/>
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5109BBC-6317-43A4-A331-8B6E954B9E7D}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,10 +1053,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1064,10 +1064,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="C5" s="3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1123,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9D608D-2646-472B-9FB7-832AE684CD5D}">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1390,7 +1390,7 @@
         <v>5</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q3:Q12" si="0">1/(1+EXP(-O4*$B$13+$B$12))</f>
+        <f t="shared" ref="Q4:Q12" si="0">1/(1+EXP(-O4*$B$13+$B$12))</f>
         <v>0.99330714907571527</v>
       </c>
       <c r="R4">
@@ -1401,16 +1401,16 @@
         <v>11</v>
       </c>
       <c r="U4" s="1">
-        <v>6.8624956952355376</v>
+        <v>13.724991390471075</v>
       </c>
       <c r="V4" s="1">
-        <v>6.8624956952355376</v>
+        <v>13.724991390471075</v>
       </c>
       <c r="W4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X4">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -1471,16 +1471,16 @@
         <v>12</v>
       </c>
       <c r="U5" s="3">
-        <v>1.8412250628948656</v>
+        <v>2.945960100631785</v>
       </c>
       <c r="V5" s="3">
-        <v>1.8412250628948656</v>
+        <v>2.945960100631785</v>
       </c>
       <c r="W5">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="X5">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented email functionality to history.py
</commit_message>
<xml_diff>
--- a/config_files/State_Conversion.xlsx
+++ b/config_files/State_Conversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsakG\projects\exjobb\config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8A673F-E55E-462D-AAE4-021CCF4B0D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC895D7-F4DD-4D69-9E8C-D04A90A4227F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31920" yWindow="3030" windowWidth="21600" windowHeight="12735" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StartingState" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>ai_ml</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Phi, Psi</t>
+  </si>
+  <si>
+    <t>Params_0_A</t>
   </si>
 </sst>
 </file>
@@ -499,17 +502,17 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B2:C12"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>30</v>
       </c>
@@ -517,7 +520,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -529,7 +532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -540,7 +543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -551,7 +554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -562,7 +565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -573,7 +576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -584,7 +587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -595,7 +598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -606,7 +609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -617,7 +620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -628,7 +631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -649,15 +652,15 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E40" sqref="E39:E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B1" t="str" cm="1">
         <f t="array" ref="B1:L1">TRANSPOSE(StartingState!A2:A12)</f>
         <v>sen_tec</v>
@@ -693,7 +696,7 @@
         <v>sim_mod</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -732,7 +735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -770,7 +773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -808,7 +811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -846,7 +849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -884,7 +887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -922,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -960,7 +963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1007,25 +1010,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5109BBC-6317-43A4-A331-8B6E954B9E7D}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1037,7 +1040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1048,7 +1051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1059,7 +1062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1070,7 +1073,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1081,7 +1084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1103,7 +1106,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1123,21 +1126,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9D608D-2646-472B-9FB7-832AE684CD5D}">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1200,7 +1203,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1273,7 +1276,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1343,7 +1346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1413,7 +1416,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1483,7 +1486,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1553,7 +1556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1623,7 +1626,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1693,7 +1696,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1763,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="N10" t="str">
         <v>com_net</v>
       </c>
@@ -1782,7 +1785,7 @@
         <v>0.99330714907571527</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="N11" t="str">
         <v>ene_mgm</v>
       </c>
@@ -1801,7 +1804,7 @@
         <v>0.2689414213699951</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1826,7 +1829,7 @@
         <v>4.7425873177566781E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1834,7 +1837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Bra hyperparametrar och custom theta_0
</commit_message>
<xml_diff>
--- a/config_files/State_Conversion.xlsx
+++ b/config_files/State_Conversion.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsakG\projects\exjobb\config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AB47A5-C530-4BF0-9C20-7BD68C1919C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D7FB55-139C-4F7D-8DEB-923410E1E8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StartingState" sheetId="14" r:id="rId1"/>
     <sheet name="ConversionMatrix" sheetId="13" r:id="rId2"/>
     <sheet name="BaseParamsPaper" sheetId="17" r:id="rId3"/>
-    <sheet name="Sammanställning" sheetId="3" r:id="rId4"/>
-    <sheet name="Svar" sheetId="1" r:id="rId5"/>
-    <sheet name="BP1" sheetId="4" r:id="rId6"/>
-    <sheet name="BP2" sheetId="9" r:id="rId7"/>
-    <sheet name="BP3" sheetId="10" r:id="rId8"/>
-    <sheet name="BP4" sheetId="11" r:id="rId9"/>
-    <sheet name="BP5" sheetId="12" r:id="rId10"/>
-    <sheet name="S0" sheetId="16" r:id="rId11"/>
-    <sheet name="_56F9DC9755BA473782653E2940F9" sheetId="2" state="veryHidden" r:id="rId12"/>
+    <sheet name="BaseParamsCustom" sheetId="18" r:id="rId4"/>
+    <sheet name="Sammanställning" sheetId="3" r:id="rId5"/>
+    <sheet name="Svar" sheetId="1" r:id="rId6"/>
+    <sheet name="BP1" sheetId="4" r:id="rId7"/>
+    <sheet name="BP2" sheetId="9" r:id="rId8"/>
+    <sheet name="BP3" sheetId="10" r:id="rId9"/>
+    <sheet name="BP4" sheetId="11" r:id="rId10"/>
+    <sheet name="BP5" sheetId="12" r:id="rId11"/>
+    <sheet name="S0" sheetId="16" r:id="rId12"/>
+    <sheet name="_56F9DC9755BA473782653E2940F9" sheetId="2" state="veryHidden" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_56F9DC9755BA473782653E2940F9FormId">"7Bg_kSZ_X0yoFnhP6aWO3SRr_qJeELtJm5w6V50Yo09URFcyMDNJRzJSVzVYQTM0NVYwSE9PQU9IQSQlQCN0PWcu"</definedName>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="137">
   <si>
     <t>PlayerA_y</t>
   </si>
@@ -1442,6 +1443,777 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F183AC-3723-8146-871E-39165557EB9D}">
+  <dimension ref="A3:O18"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3">
+        <f>SUM(COUNTIF(B7:B1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(B7:B1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(B7:B1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
+        <v>6.833333333333333</v>
+      </c>
+      <c r="C3">
+        <f>SUM(COUNTIF(C7:C1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(C7:C1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(C7:C1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
+        <v>5.083333333333333</v>
+      </c>
+      <c r="D3">
+        <f>SUM(COUNTIF(D7:D1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(D7:D1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(D7:D1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
+        <v>4.416666666666667</v>
+      </c>
+      <c r="E3">
+        <f>SUM(COUNTIF(E7:E1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(E7:E1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(E7:E1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
+        <v>4.833333333333333</v>
+      </c>
+      <c r="F3">
+        <f>SUM(COUNTIF(F7:F1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(F7:F1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(F7:F1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
+        <v>2.4166666666666665</v>
+      </c>
+      <c r="G3">
+        <f>SUM(COUNTIF(G7:G1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(G7:G1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(G7:G1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
+        <v>6.083333333333333</v>
+      </c>
+      <c r="H3">
+        <f>SUM(COUNTIF(H7:H1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(H7:H1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(H7:H1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
+        <v>5.833333333333333</v>
+      </c>
+      <c r="I3">
+        <f>SUM(COUNTIF(I7:I1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(I7:I1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(I7:I1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
+        <v>3.75</v>
+      </c>
+      <c r="J3">
+        <f>SUM(COUNTIF(J7:J1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(J7:J1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(J7:J1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
+        <v>4.916666666666667</v>
+      </c>
+      <c r="K3">
+        <f>SUM(COUNTIF(K7:K1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(K7:K1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(K7:K1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="L3">
+        <f>SUM(COUNTIF(L7:L1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(L7:L1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(L7:L1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="M3">
+        <f>SUM(COUNTIF(M7:M1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(M7:M1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(M7:M1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="N3">
+        <f>SUM(COUNTIF(N7:N1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(N7:N1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(N7:N1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
+        <v>2.8333333333333335</v>
+      </c>
+      <c r="O3">
+        <f>SUM(COUNTIF(O7:O1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(O7:O1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(O7:O1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="str" cm="1">
+        <f t="array" ref="B4">INDEX(B7:B13,MODE(MATCH(B7:B13,B7:B13,0)))</f>
+        <v>Critical</v>
+      </c>
+      <c r="C4" t="str" cm="1">
+        <f t="array" ref="C4">INDEX(C7:C13,MODE(MATCH(C7:C13,C7:C13,0)))</f>
+        <v>Critical</v>
+      </c>
+      <c r="D4" t="str" cm="1">
+        <f t="array" ref="D4">INDEX(D7:D13,MODE(MATCH(D7:D13,D7:D13,0)))</f>
+        <v>Critical</v>
+      </c>
+      <c r="E4" t="str" cm="1">
+        <f t="array" ref="E4">INDEX(E7:E13,MODE(MATCH(E7:E13,E7:E13,0)))</f>
+        <v>Major</v>
+      </c>
+      <c r="F4" t="str" cm="1">
+        <f t="array" ref="F4">INDEX(F7:F13,MODE(MATCH(F7:F13,F7:F13,0)))</f>
+        <v>Major</v>
+      </c>
+      <c r="G4" t="str" cm="1">
+        <f t="array" ref="G4">INDEX(G7:G13,MODE(MATCH(G7:G13,G7:G13,0)))</f>
+        <v>Critical</v>
+      </c>
+      <c r="H4" t="str" cm="1">
+        <f t="array" ref="H4">INDEX(H7:H13,MODE(MATCH(H7:H13,H7:H13,0)))</f>
+        <v>Major</v>
+      </c>
+      <c r="I4" t="str" cm="1">
+        <f t="array" ref="I4">INDEX(I7:I13,MODE(MATCH(I7:I13,I7:I13,0)))</f>
+        <v>Minor</v>
+      </c>
+      <c r="J4" t="str" cm="1">
+        <f t="array" ref="J4">INDEX(J7:J13,MODE(MATCH(J7:J13,J7:J13,0)))</f>
+        <v>Major</v>
+      </c>
+      <c r="K4" t="str" cm="1">
+        <f t="array" ref="K4">INDEX(K7:K13,MODE(MATCH(K7:K13,K7:K13,0)))</f>
+        <v>Minor</v>
+      </c>
+      <c r="L4" t="str" cm="1">
+        <f t="array" ref="L4">INDEX(L7:L13,MODE(MATCH(L7:L13,L7:L13,0)))</f>
+        <v>Critical</v>
+      </c>
+      <c r="M4" t="str" cm="1">
+        <f t="array" ref="M4">INDEX(M7:M13,MODE(MATCH(M7:M13,M7:M13,0)))</f>
+        <v>Minor</v>
+      </c>
+      <c r="N4" t="str" cm="1">
+        <f t="array" ref="N4">INDEX(N7:N13,MODE(MATCH(N7:N13,N7:N13,0)))</f>
+        <v>Minor</v>
+      </c>
+      <c r="O4" t="str" cm="1">
+        <f t="array" ref="O4">INDEX(O7:O13,MODE(MATCH(O7:O13,O7:O13,0)))</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" cm="1">
+        <f t="array" ref="B5">VLOOKUP(INDEX(B7:B13,MODE(MATCH(B7:B13,B7:B13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="C5" cm="1">
+        <f t="array" ref="C5">VLOOKUP(INDEX(C7:C13,MODE(MATCH(C7:C13,C7:C13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="D5" cm="1">
+        <f t="array" ref="D5">VLOOKUP(INDEX(D7:D13,MODE(MATCH(D7:D13,D7:D13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="E5" cm="1">
+        <f t="array" ref="E5">VLOOKUP(INDEX(E7:E13,MODE(MATCH(E7:E13,E7:E13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="F5" cm="1">
+        <f t="array" ref="F5">VLOOKUP(INDEX(F7:F13,MODE(MATCH(F7:F13,F7:F13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="G5" cm="1">
+        <f t="array" ref="G5">VLOOKUP(INDEX(G7:G13,MODE(MATCH(G7:G13,G7:G13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="H5" cm="1">
+        <f t="array" ref="H5">VLOOKUP(INDEX(H7:H13,MODE(MATCH(H7:H13,H7:H13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="I5" cm="1">
+        <f t="array" ref="I5">VLOOKUP(INDEX(I7:I13,MODE(MATCH(I7:I13,I7:I13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J5" cm="1">
+        <f t="array" ref="J5">VLOOKUP(INDEX(J7:J13,MODE(MATCH(J7:J13,J7:J13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="K5" cm="1">
+        <f t="array" ref="K5">VLOOKUP(INDEX(K7:K13,MODE(MATCH(K7:K13,K7:K13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="L5" cm="1">
+        <f t="array" ref="L5">VLOOKUP(INDEX(L7:L13,MODE(MATCH(L7:L13,L7:L13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="M5" cm="1">
+        <f t="array" ref="M5">VLOOKUP(INDEX(M7:M13,MODE(MATCH(M7:M13,M7:M13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N5" cm="1">
+        <f t="array" ref="N5">VLOOKUP(INDEX(N7:N13,MODE(MATCH(N7:N13,N7:N13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="O5" cm="1">
+        <f t="array" ref="O5">VLOOKUP(INDEX(O7:O13,MODE(MATCH(O7:O13,O7:O13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="str" cm="1">
+        <f t="array" ref="B6:O18">Svar[[#All],[Sensor Technology4]:[Ethics and Regulations4]]</f>
+        <v>Sensor Technology4</v>
+      </c>
+      <c r="C6" s="3" t="str">
+        <v>Collaborative systems4</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <v>Technologies enabling mobility4</v>
+      </c>
+      <c r="E6" s="3" t="str">
+        <v>Control systems and algorithms4</v>
+      </c>
+      <c r="F6" s="3" t="str">
+        <v>Localization and mapping4</v>
+      </c>
+      <c r="G6" s="3" t="str">
+        <v>Sensor Fusion4</v>
+      </c>
+      <c r="H6" s="3" t="str">
+        <v>AI and Machine Learning4</v>
+      </c>
+      <c r="I6" s="3" t="str">
+        <v>Edge computing4</v>
+      </c>
+      <c r="J6" s="3" t="str">
+        <v>Communications and networking4</v>
+      </c>
+      <c r="K6" s="3" t="str">
+        <v>Energy Management4</v>
+      </c>
+      <c r="L6" s="3" t="str">
+        <v>Simulation and modeling4</v>
+      </c>
+      <c r="M6" s="3" t="str">
+        <v>Human Machine Interaction4</v>
+      </c>
+      <c r="N6" s="3" t="str">
+        <v>Cybersecurity4</v>
+      </c>
+      <c r="O6" s="3" t="str">
+        <v>Ethics and Regulations4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="D7" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="F7" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="H7" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="I7" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Major</v>
+      </c>
+      <c r="K7" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="L7" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="M7" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="N7" t="str">
+        <v>Major</v>
+      </c>
+      <c r="O7" t="str">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Major</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="H8" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="I8" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="K8" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="L8" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="M8" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="N8" t="str">
+        <v>Major</v>
+      </c>
+      <c r="O8" t="str">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Major</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Major</v>
+      </c>
+      <c r="H9" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="I9" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="K9" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="L9" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="M9" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N9" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O9" t="str">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="str">
+        <v>Major</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Major</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Major</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Major</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="str">
+        <v>Major</v>
+      </c>
+      <c r="I10" t="str">
+        <v>Major</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Major</v>
+      </c>
+      <c r="K10" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="L10" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="M10" t="str">
+        <v>Major</v>
+      </c>
+      <c r="N10" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="O10" t="str">
+        <v>Minor</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="str">
+        <v>Major</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Major</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Major</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="G11" t="str">
+        <v>Major</v>
+      </c>
+      <c r="H11" t="str">
+        <v>Major</v>
+      </c>
+      <c r="I11" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="J11" t="str">
+        <v>Major</v>
+      </c>
+      <c r="K11" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="L11" t="str">
+        <v>Major</v>
+      </c>
+      <c r="M11" t="str">
+        <v>Major</v>
+      </c>
+      <c r="N11" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="O11" t="str">
+        <v>Major</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Major</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Major</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Major</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="G12" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="H12" t="str">
+        <v>Major</v>
+      </c>
+      <c r="I12" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="J12" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="K12" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="L12" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="M12" t="str">
+        <v>Major</v>
+      </c>
+      <c r="N12" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="O12" t="str">
+        <v>Minor</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Major</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Major</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Major</v>
+      </c>
+      <c r="G13" t="str">
+        <v>Major</v>
+      </c>
+      <c r="H13" t="str">
+        <v>Major</v>
+      </c>
+      <c r="I13" t="str">
+        <v>Major</v>
+      </c>
+      <c r="J13" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="K13" t="str">
+        <v>Major</v>
+      </c>
+      <c r="L13" t="str">
+        <v>Major</v>
+      </c>
+      <c r="M13" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="N13" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="O13" t="str">
+        <v>Minor</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
+        <v>Major</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Major</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="G14" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="H14" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="I14" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="J14" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="K14" t="str">
+        <v>Major</v>
+      </c>
+      <c r="L14" t="str">
+        <v>Major</v>
+      </c>
+      <c r="M14" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="N14" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="O14" t="str">
+        <v>Major</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Major</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="F15" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="H15" t="str">
+        <v>Major</v>
+      </c>
+      <c r="I15" t="str">
+        <v>Major</v>
+      </c>
+      <c r="J15" t="str">
+        <v>Major</v>
+      </c>
+      <c r="K15" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="L15" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="M15" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="N15" t="str">
+        <v>Major</v>
+      </c>
+      <c r="O15" t="str">
+        <v>Minor</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="C16" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Major</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="F16" t="str">
+        <v>Major</v>
+      </c>
+      <c r="G16" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="H16" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="I16" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="J16" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="K16" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="L16" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="M16" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N16" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="O16" t="str">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Major</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Major</v>
+      </c>
+      <c r="F17" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="G17" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="H17" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="I17" t="str">
+        <v>Major</v>
+      </c>
+      <c r="J17" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="K17" t="str">
+        <v>Major</v>
+      </c>
+      <c r="L17" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="M17" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="N17" t="str">
+        <v>Major</v>
+      </c>
+      <c r="O17" t="str">
+        <v>Minor</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Major</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Major</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Major</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="G18" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="H18" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="I18" t="str">
+        <v>Major</v>
+      </c>
+      <c r="J18" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="K18" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="L18" t="str">
+        <v>Minor</v>
+      </c>
+      <c r="M18" t="str">
+        <v>Major</v>
+      </c>
+      <c r="N18" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="O18" t="str">
+        <v>Minor</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A95E2E-9D2C-344A-9A72-B68EBF9A12CE}">
   <dimension ref="A3:O18"/>
   <sheetViews>
@@ -2212,7 +2984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8558BD-5754-C44D-9492-8D7ECAF963BA}">
   <dimension ref="A3:O39"/>
   <sheetViews>
@@ -3242,7 +4014,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -3799,7 +4571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968E2FB3-FF17-438C-AFFB-76D4B50D10E5}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -3910,6 +4682,120 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EA64B1-B95A-4F85-BBC4-7B4E1FF484C7}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>2.8780000000000001</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>2</v>
+      </c>
+      <c r="B6" s="7">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <f>2.878</f>
+        <v>2.8780000000000001</v>
+      </c>
+      <c r="B7" s="6">
+        <f>2.878</f>
+        <v>2.8780000000000001</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E9EE980-847C-462B-AF52-914991B73E1E}">
   <dimension ref="B1:P25"/>
   <sheetViews>
@@ -4600,7 +5486,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:CK15"/>
   <sheetViews>
@@ -8077,7 +8963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3FDF05-311E-3742-822F-51D4637E4B5B}">
   <dimension ref="A3:O18"/>
   <sheetViews>
@@ -8848,7 +9734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC38DDE5-AFA9-464C-AABF-A685E70C75BE}">
   <dimension ref="A3:O18"/>
   <sheetViews>
@@ -9619,7 +10505,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F4AC626-133A-F74F-9EAA-8F3B2E6E439C}">
   <dimension ref="A3:O18"/>
   <sheetViews>
@@ -10390,789 +11276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F183AC-3723-8146-871E-39165557EB9D}">
-  <dimension ref="A3:O18"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3">
-        <f>SUM(COUNTIF(B7:B1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(B7:B1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(B7:B1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
-        <v>6.833333333333333</v>
-      </c>
-      <c r="C3">
-        <f>SUM(COUNTIF(C7:C1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(C7:C1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(C7:C1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
-        <v>5.083333333333333</v>
-      </c>
-      <c r="D3">
-        <f>SUM(COUNTIF(D7:D1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(D7:D1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(D7:D1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
-        <v>4.416666666666667</v>
-      </c>
-      <c r="E3">
-        <f>SUM(COUNTIF(E7:E1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(E7:E1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(E7:E1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
-        <v>4.833333333333333</v>
-      </c>
-      <c r="F3">
-        <f>SUM(COUNTIF(F7:F1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(F7:F1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(F7:F1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
-        <v>2.4166666666666665</v>
-      </c>
-      <c r="G3">
-        <f>SUM(COUNTIF(G7:G1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(G7:G1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(G7:G1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
-        <v>6.083333333333333</v>
-      </c>
-      <c r="H3">
-        <f>SUM(COUNTIF(H7:H1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(H7:H1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(H7:H1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
-        <v>5.833333333333333</v>
-      </c>
-      <c r="I3">
-        <f>SUM(COUNTIF(I7:I1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(I7:I1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(I7:I1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
-        <v>3.75</v>
-      </c>
-      <c r="J3">
-        <f>SUM(COUNTIF(J7:J1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(J7:J1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(J7:J1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
-        <v>4.916666666666667</v>
-      </c>
-      <c r="K3">
-        <f>SUM(COUNTIF(K7:K1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(K7:K1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(K7:K1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="L3">
-        <f>SUM(COUNTIF(L7:L1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(L7:L1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(L7:L1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
-        <v>2.6666666666666665</v>
-      </c>
-      <c r="M3">
-        <f>SUM(COUNTIF(M7:M1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(M7:M1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(M7:M1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
-        <v>2.1666666666666665</v>
-      </c>
-      <c r="N3">
-        <f>SUM(COUNTIF(N7:N1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(N7:N1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(N7:N1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
-        <v>2.8333333333333335</v>
-      </c>
-      <c r="O3">
-        <f>SUM(COUNTIF(O7:O1048576,Sammanställning!$N$3)*Sammanställning!$O$3,COUNTIF(O7:O1048576,Sammanställning!$N$4)*Sammanställning!$O$4,COUNTIF(O7:O1048576,Sammanställning!$N$5)*Sammanställning!$O$5)/Sammanställning!$O$9</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" t="str" cm="1">
-        <f t="array" ref="B4">INDEX(B7:B13,MODE(MATCH(B7:B13,B7:B13,0)))</f>
-        <v>Critical</v>
-      </c>
-      <c r="C4" t="str" cm="1">
-        <f t="array" ref="C4">INDEX(C7:C13,MODE(MATCH(C7:C13,C7:C13,0)))</f>
-        <v>Critical</v>
-      </c>
-      <c r="D4" t="str" cm="1">
-        <f t="array" ref="D4">INDEX(D7:D13,MODE(MATCH(D7:D13,D7:D13,0)))</f>
-        <v>Critical</v>
-      </c>
-      <c r="E4" t="str" cm="1">
-        <f t="array" ref="E4">INDEX(E7:E13,MODE(MATCH(E7:E13,E7:E13,0)))</f>
-        <v>Major</v>
-      </c>
-      <c r="F4" t="str" cm="1">
-        <f t="array" ref="F4">INDEX(F7:F13,MODE(MATCH(F7:F13,F7:F13,0)))</f>
-        <v>Major</v>
-      </c>
-      <c r="G4" t="str" cm="1">
-        <f t="array" ref="G4">INDEX(G7:G13,MODE(MATCH(G7:G13,G7:G13,0)))</f>
-        <v>Critical</v>
-      </c>
-      <c r="H4" t="str" cm="1">
-        <f t="array" ref="H4">INDEX(H7:H13,MODE(MATCH(H7:H13,H7:H13,0)))</f>
-        <v>Major</v>
-      </c>
-      <c r="I4" t="str" cm="1">
-        <f t="array" ref="I4">INDEX(I7:I13,MODE(MATCH(I7:I13,I7:I13,0)))</f>
-        <v>Minor</v>
-      </c>
-      <c r="J4" t="str" cm="1">
-        <f t="array" ref="J4">INDEX(J7:J13,MODE(MATCH(J7:J13,J7:J13,0)))</f>
-        <v>Major</v>
-      </c>
-      <c r="K4" t="str" cm="1">
-        <f t="array" ref="K4">INDEX(K7:K13,MODE(MATCH(K7:K13,K7:K13,0)))</f>
-        <v>Minor</v>
-      </c>
-      <c r="L4" t="str" cm="1">
-        <f t="array" ref="L4">INDEX(L7:L13,MODE(MATCH(L7:L13,L7:L13,0)))</f>
-        <v>Critical</v>
-      </c>
-      <c r="M4" t="str" cm="1">
-        <f t="array" ref="M4">INDEX(M7:M13,MODE(MATCH(M7:M13,M7:M13,0)))</f>
-        <v>Minor</v>
-      </c>
-      <c r="N4" t="str" cm="1">
-        <f t="array" ref="N4">INDEX(N7:N13,MODE(MATCH(N7:N13,N7:N13,0)))</f>
-        <v>Minor</v>
-      </c>
-      <c r="O4" t="str" cm="1">
-        <f t="array" ref="O4">INDEX(O7:O13,MODE(MATCH(O7:O13,O7:O13,0)))</f>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" cm="1">
-        <f t="array" ref="B5">VLOOKUP(INDEX(B7:B13,MODE(MATCH(B7:B13,B7:B13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
-        <v>9</v>
-      </c>
-      <c r="C5" cm="1">
-        <f t="array" ref="C5">VLOOKUP(INDEX(C7:C13,MODE(MATCH(C7:C13,C7:C13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
-        <v>9</v>
-      </c>
-      <c r="D5" cm="1">
-        <f t="array" ref="D5">VLOOKUP(INDEX(D7:D13,MODE(MATCH(D7:D13,D7:D13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
-        <v>9</v>
-      </c>
-      <c r="E5" cm="1">
-        <f t="array" ref="E5">VLOOKUP(INDEX(E7:E13,MODE(MATCH(E7:E13,E7:E13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="F5" cm="1">
-        <f t="array" ref="F5">VLOOKUP(INDEX(F7:F13,MODE(MATCH(F7:F13,F7:F13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="G5" cm="1">
-        <f t="array" ref="G5">VLOOKUP(INDEX(G7:G13,MODE(MATCH(G7:G13,G7:G13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
-        <v>9</v>
-      </c>
-      <c r="H5" cm="1">
-        <f t="array" ref="H5">VLOOKUP(INDEX(H7:H13,MODE(MATCH(H7:H13,H7:H13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="I5" cm="1">
-        <f t="array" ref="I5">VLOOKUP(INDEX(I7:I13,MODE(MATCH(I7:I13,I7:I13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="J5" cm="1">
-        <f t="array" ref="J5">VLOOKUP(INDEX(J7:J13,MODE(MATCH(J7:J13,J7:J13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="K5" cm="1">
-        <f t="array" ref="K5">VLOOKUP(INDEX(K7:K13,MODE(MATCH(K7:K13,K7:K13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="L5" cm="1">
-        <f t="array" ref="L5">VLOOKUP(INDEX(L7:L13,MODE(MATCH(L7:L13,L7:L13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
-        <v>9</v>
-      </c>
-      <c r="M5" cm="1">
-        <f t="array" ref="M5">VLOOKUP(INDEX(M7:M13,MODE(MATCH(M7:M13,M7:M13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="N5" cm="1">
-        <f t="array" ref="N5">VLOOKUP(INDEX(N7:N13,MODE(MATCH(N7:N13,N7:N13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="O5" cm="1">
-        <f t="array" ref="O5">VLOOKUP(INDEX(O7:O13,MODE(MATCH(O7:O13,O7:O13,0))),Sammanställning!$N$2:$O$5,2,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="str" cm="1">
-        <f t="array" ref="B6:O18">Svar[[#All],[Sensor Technology4]:[Ethics and Regulations4]]</f>
-        <v>Sensor Technology4</v>
-      </c>
-      <c r="C6" s="3" t="str">
-        <v>Collaborative systems4</v>
-      </c>
-      <c r="D6" s="3" t="str">
-        <v>Technologies enabling mobility4</v>
-      </c>
-      <c r="E6" s="3" t="str">
-        <v>Control systems and algorithms4</v>
-      </c>
-      <c r="F6" s="3" t="str">
-        <v>Localization and mapping4</v>
-      </c>
-      <c r="G6" s="3" t="str">
-        <v>Sensor Fusion4</v>
-      </c>
-      <c r="H6" s="3" t="str">
-        <v>AI and Machine Learning4</v>
-      </c>
-      <c r="I6" s="3" t="str">
-        <v>Edge computing4</v>
-      </c>
-      <c r="J6" s="3" t="str">
-        <v>Communications and networking4</v>
-      </c>
-      <c r="K6" s="3" t="str">
-        <v>Energy Management4</v>
-      </c>
-      <c r="L6" s="3" t="str">
-        <v>Simulation and modeling4</v>
-      </c>
-      <c r="M6" s="3" t="str">
-        <v>Human Machine Interaction4</v>
-      </c>
-      <c r="N6" s="3" t="str">
-        <v>Cybersecurity4</v>
-      </c>
-      <c r="O6" s="3" t="str">
-        <v>Ethics and Regulations4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="D7" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="F7" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="G7" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="H7" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="I7" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="J7" t="str">
-        <v>Major</v>
-      </c>
-      <c r="K7" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="L7" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="M7" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="N7" t="str">
-        <v>Major</v>
-      </c>
-      <c r="O7" t="str">
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="D8" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="E8" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="F8" t="str">
-        <v>Major</v>
-      </c>
-      <c r="G8" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="H8" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="I8" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="J8" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="K8" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="L8" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="M8" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="N8" t="str">
-        <v>Major</v>
-      </c>
-      <c r="O8" t="str">
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="D9" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="E9" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="F9" t="str">
-        <v>Major</v>
-      </c>
-      <c r="G9" t="str">
-        <v>Major</v>
-      </c>
-      <c r="H9" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="I9" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="J9" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="K9" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="L9" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="M9" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="N9" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="O9" t="str">
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" t="str">
-        <v>Major</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Major</v>
-      </c>
-      <c r="D10" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="E10" t="str">
-        <v>Major</v>
-      </c>
-      <c r="F10" t="str">
-        <v>Major</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" t="str">
-        <v>Major</v>
-      </c>
-      <c r="I10" t="str">
-        <v>Major</v>
-      </c>
-      <c r="J10" t="str">
-        <v>Major</v>
-      </c>
-      <c r="K10" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="L10" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="M10" t="str">
-        <v>Major</v>
-      </c>
-      <c r="N10" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="O10" t="str">
-        <v>Minor</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" t="str">
-        <v>Major</v>
-      </c>
-      <c r="C11" t="str">
-        <v>Major</v>
-      </c>
-      <c r="D11" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="E11" t="str">
-        <v>Major</v>
-      </c>
-      <c r="F11" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="G11" t="str">
-        <v>Major</v>
-      </c>
-      <c r="H11" t="str">
-        <v>Major</v>
-      </c>
-      <c r="I11" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="J11" t="str">
-        <v>Major</v>
-      </c>
-      <c r="K11" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="L11" t="str">
-        <v>Major</v>
-      </c>
-      <c r="M11" t="str">
-        <v>Major</v>
-      </c>
-      <c r="N11" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="O11" t="str">
-        <v>Major</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B12" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Major</v>
-      </c>
-      <c r="D12" t="str">
-        <v>Major</v>
-      </c>
-      <c r="E12" t="str">
-        <v>Major</v>
-      </c>
-      <c r="F12" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="G12" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="H12" t="str">
-        <v>Major</v>
-      </c>
-      <c r="I12" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="J12" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="K12" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="L12" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="M12" t="str">
-        <v>Major</v>
-      </c>
-      <c r="N12" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="O12" t="str">
-        <v>Minor</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="C13" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="D13" t="str">
-        <v>Major</v>
-      </c>
-      <c r="E13" t="str">
-        <v>Major</v>
-      </c>
-      <c r="F13" t="str">
-        <v>Major</v>
-      </c>
-      <c r="G13" t="str">
-        <v>Major</v>
-      </c>
-      <c r="H13" t="str">
-        <v>Major</v>
-      </c>
-      <c r="I13" t="str">
-        <v>Major</v>
-      </c>
-      <c r="J13" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="K13" t="str">
-        <v>Major</v>
-      </c>
-      <c r="L13" t="str">
-        <v>Major</v>
-      </c>
-      <c r="M13" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="N13" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="O13" t="str">
-        <v>Minor</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" t="str">
-        <v>Major</v>
-      </c>
-      <c r="C14" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="D14" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="E14" t="str">
-        <v>Major</v>
-      </c>
-      <c r="F14" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="G14" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="H14" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="I14" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="J14" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="K14" t="str">
-        <v>Major</v>
-      </c>
-      <c r="L14" t="str">
-        <v>Major</v>
-      </c>
-      <c r="M14" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="N14" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="O14" t="str">
-        <v>Major</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="C15" t="str">
-        <v>Major</v>
-      </c>
-      <c r="D15" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="E15" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="F15" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="G15" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="H15" t="str">
-        <v>Major</v>
-      </c>
-      <c r="I15" t="str">
-        <v>Major</v>
-      </c>
-      <c r="J15" t="str">
-        <v>Major</v>
-      </c>
-      <c r="K15" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="L15" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="M15" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="N15" t="str">
-        <v>Major</v>
-      </c>
-      <c r="O15" t="str">
-        <v>Minor</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="C16" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="D16" t="str">
-        <v>Major</v>
-      </c>
-      <c r="E16" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="F16" t="str">
-        <v>Major</v>
-      </c>
-      <c r="G16" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="H16" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="I16" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="J16" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="K16" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="L16" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="M16" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="N16" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="O16" t="str">
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="C17" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="D17" t="str">
-        <v>Major</v>
-      </c>
-      <c r="E17" t="str">
-        <v>Major</v>
-      </c>
-      <c r="F17" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="G17" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="H17" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="I17" t="str">
-        <v>Major</v>
-      </c>
-      <c r="J17" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="K17" t="str">
-        <v>Major</v>
-      </c>
-      <c r="L17" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="M17" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="N17" t="str">
-        <v>Major</v>
-      </c>
-      <c r="O17" t="str">
-        <v>Minor</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="C18" t="str">
-        <v>Major</v>
-      </c>
-      <c r="D18" t="str">
-        <v>Major</v>
-      </c>
-      <c r="E18" t="str">
-        <v>Major</v>
-      </c>
-      <c r="F18" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="G18" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="H18" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="I18" t="str">
-        <v>Major</v>
-      </c>
-      <c r="J18" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="K18" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="L18" t="str">
-        <v>Minor</v>
-      </c>
-      <c r="M18" t="str">
-        <v>Major</v>
-      </c>
-      <c r="N18" t="str">
-        <v>Critical</v>
-      </c>
-      <c r="O18" t="str">
-        <v>Minor</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dc4417ab-57e7-4e1c-9da8-e07bf8fce2aa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a6949cbf-6185-4000-ad09-6ccd2758cad5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -11181,7 +11285,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100C3B21DCB732F554E987E9492B21347DB" ma:contentTypeVersion="10" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="bfbc4f1336637a71548d0312365bfd65">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dc4417ab-57e7-4e1c-9da8-e07bf8fce2aa" xmlns:ns3="a6949cbf-6185-4000-ad09-6ccd2758cad5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a9fc7021594913e7ea907481551a91b" ns2:_="" ns3:_="">
     <xsd:import namespace="dc4417ab-57e7-4e1c-9da8-e07bf8fce2aa"/>
@@ -11386,18 +11490,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60013D14-2CBB-4465-8219-EFB55907661B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dc4417ab-57e7-4e1c-9da8-e07bf8fce2aa"/>
-    <ds:schemaRef ds:uri="a6949cbf-6185-4000-ad09-6ccd2758cad5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dc4417ab-57e7-4e1c-9da8-e07bf8fce2aa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a6949cbf-6185-4000-ad09-6ccd2758cad5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B76B859D-A811-4493-84DA-CB431A622007}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -11405,7 +11509,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3FDB04A-9560-4CE6-9E67-F5F28406E0F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11422,4 +11526,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60013D14-2CBB-4465-8219-EFB55907661B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dc4417ab-57e7-4e1c-9da8-e07bf8fce2aa"/>
+    <ds:schemaRef ds:uri="a6949cbf-6185-4000-ad09-6ccd2758cad5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>